<commit_message>
create entity etrm etrs
</commit_message>
<xml_diff>
--- a/testData/CreateEntity/CreateEntity_ETRS_NewValues_Test.xlsx
+++ b/testData/CreateEntity/CreateEntity_ETRS_NewValues_Test.xlsx
@@ -14,7 +14,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="112">
   <si>
     <t>WorflowName</t>
   </si>
@@ -219,9 +219,6 @@
     <t>Steven</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Add New Text</t>
   </si>
   <si>
@@ -318,9 +315,6 @@
     <t>Test Enquiry Text Area</t>
   </si>
   <si>
-    <t>2024-06-04</t>
-  </si>
-  <si>
     <t>wfCreateEntity_ETRS</t>
   </si>
   <si>
@@ -333,47 +327,43 @@
     <t>6</t>
   </si>
   <si>
-    <t>02:35:55 PM</t>
-  </si>
-  <si>
-    <t>2024-06-07 05:00:00 PM</t>
-  </si>
-  <si>
-    <t>CT: Tue, Jun 04, 2024 at 6:05 PM</t>
-  </si>
-  <si>
-    <t>CT: Tue, Jun 04, 2024 at 6:12 PM</t>
-  </si>
-  <si>
-    <t>8599228759</t>
-  </si>
-  <si>
-    <t>0685500189</t>
-  </si>
-  <si>
-    <t>6692474599</t>
-  </si>
-  <si>
-    <t>7953834762</t>
-  </si>
-  <si>
-    <t>7808175405</t>
-  </si>
-  <si>
-    <t>9996067070</t>
-  </si>
-  <si>
-    <t>3397955376</t>
-  </si>
-  <si>
-    <t>6708146757</t>
+    <t>2024-06-05</t>
+  </si>
+  <si>
+    <t>02:35:55 AM</t>
+  </si>
+  <si>
+    <t>2024-06-08 05:00:00 PM</t>
+  </si>
+  <si>
+    <t>9016402530</t>
+  </si>
+  <si>
+    <t>6532577817</t>
+  </si>
+  <si>
+    <t>5932577499</t>
+  </si>
+  <si>
+    <t>9639914330</t>
+  </si>
+  <si>
+    <t>CT: Wed, Jun 05, 2024 at 11:15 AM</t>
+  </si>
+  <si>
+    <t>CT: Wed, Jun 05, 2024 at 11:22 AM</t>
+  </si>
+  <si>
+    <t>CT: Wed, Jun 05, 2024 at 11:29 AM</t>
+  </si>
+  <si>
+    <t>CT: Wed, Jun 05, 2024 at 11:37 AM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -725,69 +715,69 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BB2"/>
   <sheetViews>
-    <sheetView topLeftCell="AK1" workbookViewId="0">
-      <selection activeCell="AS2" sqref="AS2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="18.0"/>
-    <col min="2" max="2" customWidth="true" style="2" width="22.26953125"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="29.81640625"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="11.1796875"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="26.54296875"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="13.54296875"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="14.0"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="16.453125"/>
-    <col min="9" max="9" style="2" width="8.7265625"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="12.54296875"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="11.81640625"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="9.54296875"/>
-    <col min="13" max="14" style="2" width="8.7265625"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="2" width="10.1796875"/>
-    <col min="16" max="16" style="2" width="8.7265625"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="2" width="15.1796875"/>
-    <col min="18" max="19" bestFit="true" customWidth="true" style="2" width="13.54296875"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="2" width="10.453125"/>
-    <col min="21" max="21" style="2" width="8.7265625"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="2" width="11.81640625"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="2" width="8.26953125"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="2" width="22.0"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="2" width="15.7265625"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="2" width="13.1796875"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="2" width="12.7265625"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="2" width="23.1796875"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="2" width="23.453125"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="2" width="11.7265625"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="2" width="13.1796875"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="2" width="20.453125"/>
-    <col min="33" max="33" customWidth="true" style="2" width="20.453125"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" style="2" width="18.54296875"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" style="2" width="31.26953125"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" style="2" width="21.1796875"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" style="2" width="11.81640625"/>
-    <col min="38" max="40" bestFit="true" customWidth="true" style="2" width="17.81640625"/>
-    <col min="41" max="43" bestFit="true" customWidth="true" style="2" width="10.1796875"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" style="2" width="18.453125"/>
-    <col min="45" max="45" customWidth="true" style="2" width="18.453125"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" style="2" width="18.0"/>
-    <col min="47" max="47" customWidth="true" style="2" width="18.0"/>
-    <col min="48" max="48" bestFit="true" customWidth="true" style="2" width="10.81640625"/>
-    <col min="49" max="49" bestFit="true" customWidth="true" style="2" width="10.26953125"/>
-    <col min="50" max="50" bestFit="true" customWidth="true" style="2" width="10.81640625"/>
-    <col min="51" max="51" bestFit="true" customWidth="true" style="2" width="14.1796875"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" style="2" width="10.81640625"/>
-    <col min="53" max="53" bestFit="true" customWidth="true" style="2" width="22.7265625"/>
-    <col min="54" max="54" bestFit="true" customWidth="true" style="2" width="30.26953125"/>
-    <col min="55" max="16384" style="2" width="8.7265625"/>
+    <col min="1" max="1" width="18" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.26953125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="29.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7265625" style="2"/>
+    <col min="10" max="10" width="12.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="8.7265625" style="2"/>
+    <col min="15" max="15" width="10.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.7265625" style="2"/>
+    <col min="17" max="17" width="15.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="13.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.7265625" style="2"/>
+    <col min="22" max="22" width="11.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="22" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="23.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="23.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="20.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="20.453125" style="2" customWidth="1"/>
+    <col min="34" max="34" width="18.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="31.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="21.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="38" max="40" width="17.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="41" max="43" width="10.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="18.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="18.453125" style="2" customWidth="1"/>
+    <col min="46" max="46" width="18" style="2" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="18" style="2" customWidth="1"/>
+    <col min="48" max="48" width="10.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="10.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="14.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="10.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="22.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="30.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="55" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -913,10 +903,10 @@
         <v>47</v>
       </c>
       <c r="AR1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AS1" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="AS1" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="AT1" s="2" t="s">
         <v>49</v>
@@ -943,33 +933,33 @@
         <v>56</v>
       </c>
       <c r="BB1" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G2" t="s" s="2">
-        <v>111</v>
+      <c r="G2" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I2" s="2">
         <v>3</v>
@@ -990,16 +980,16 @@
         <v>25</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="P2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="Q2" s="2" t="s">
-        <v>104</v>
-      </c>
       <c r="R2" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>44</v>
@@ -1023,46 +1013,46 @@
         <v>48</v>
       </c>
       <c r="Z2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA2" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AB2" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="AB2" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="AC2" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="AE2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AF2" t="s" s="2">
-        <v>112</v>
+      <c r="AF2" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="AG2" s="2" t="s">
         <v>40</v>
       </c>
       <c r="AH2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="AK2" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="AI2" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="AJ2" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="AK2" t="s" s="2">
-        <v>102</v>
-      </c>
       <c r="AR2" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AS2" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AT2" s="2" t="s">
         <v>50</v>
@@ -1070,26 +1060,26 @@
       <c r="AU2" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AV2" t="s" s="2">
-        <v>113</v>
+      <c r="AV2" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="AW2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="AX2" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="AX2" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="AY2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AZ2" t="s" s="2">
-        <v>114</v>
+      <c r="AZ2" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="BA2" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="BB2" s="2" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1115,62 +1105,62 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="22.26953125"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="20.453125"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="29.26953125"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="26.453125"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="16.54296875"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="13.54296875"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="16.453125"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="23.81640625"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="11.1796875"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="11.81640625"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="9.54296875"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="7.453125"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="8.81640625"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="10.1796875"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="2" width="8.1796875"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="18.453125"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="2" width="13.54296875"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="2" width="11.0"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="2" width="10.453125"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="2" width="8.54296875"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="2" width="11.81640625"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="2" width="8.26953125"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="2" width="22.0"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="2" width="15.7265625"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="2" width="13.1796875"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="2" width="19.453125"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="2" width="23.1796875"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="2" width="19.81640625"/>
-    <col min="29" max="29" customWidth="true" style="2" width="38.26953125"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="2" width="13.1796875"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="2" width="20.453125"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="2" width="15.54296875"/>
-    <col min="33" max="34" bestFit="true" customWidth="true" style="2" width="24.81640625"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" style="2" width="28.81640625"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" style="2" width="20.6328125"/>
-    <col min="37" max="39" bestFit="true" customWidth="true" style="2" width="15.54296875"/>
-    <col min="40" max="42" bestFit="true" customWidth="true" style="2" width="10.1796875"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" style="2" width="18.453125"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" style="2" width="18.0"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" style="2" width="13.81640625"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" style="2" width="10.81640625"/>
-    <col min="47" max="47" bestFit="true" customWidth="true" style="2" width="18.81640625"/>
-    <col min="48" max="48" bestFit="true" customWidth="true" style="2" width="10.81640625"/>
-    <col min="49" max="49" bestFit="true" customWidth="true" style="2" width="14.1796875"/>
-    <col min="50" max="50" bestFit="true" customWidth="true" style="2" width="10.81640625"/>
-    <col min="51" max="51" bestFit="true" customWidth="true" style="2" width="12.81640625"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" style="2" width="16.7265625"/>
-    <col min="53" max="16384" style="2" width="8.7265625"/>
+    <col min="1" max="1" width="22.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="22" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="19.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="38.26953125" style="2" customWidth="1"/>
+    <col min="30" max="30" width="13.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="20.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="34" width="24.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="28.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="20.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="37" max="39" width="15.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="40" max="42" width="10.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="18.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="18" style="2" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="13.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="10.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="18.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="10.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="14.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="10.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="12.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="16.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="53" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -1296,10 +1286,10 @@
         <v>47</v>
       </c>
       <c r="AR1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AS1" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="AS1" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="AT1" s="2" t="s">
         <v>49</v>
@@ -1326,33 +1316,33 @@
         <v>56</v>
       </c>
       <c r="BB1" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G2" t="s" s="2">
-        <v>111</v>
+      <c r="G2" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I2" s="2">
         <v>3</v>
@@ -1373,16 +1363,16 @@
         <v>25</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="P2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="Q2" s="2" t="s">
-        <v>104</v>
-      </c>
       <c r="R2" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>44</v>
@@ -1394,7 +1384,7 @@
         <v>64</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="W2" s="7">
         <v>10000</v>
@@ -1406,46 +1396,46 @@
         <v>48</v>
       </c>
       <c r="Z2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA2" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AB2" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="AB2" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="AC2" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="AE2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AF2" t="s" s="2">
-        <v>112</v>
+      <c r="AF2" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="AG2" s="2" t="s">
         <v>40</v>
       </c>
       <c r="AH2" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="AI2" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AJ2" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="AL2" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AR2" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AS2" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AT2" s="2" t="s">
         <v>50</v>
@@ -1453,26 +1443,26 @@
       <c r="AU2" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AV2" t="s" s="2">
-        <v>113</v>
+      <c r="AV2" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="AW2" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AX2" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AY2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AZ2" t="s" s="2">
-        <v>114</v>
+      <c r="AZ2" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="BA2" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="BB2" s="2" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1497,60 +1487,60 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="22.26953125"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="20.453125"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" style="2" width="11.1796875"/>
-    <col min="5" max="6" bestFit="true" customWidth="true" style="2" width="13.54296875"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="16.453125"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="6.7265625"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="11.1796875"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="11.81640625"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="9.54296875"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="7.453125"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="8.81640625"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="10.1796875"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="2" width="8.1796875"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="18.453125"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="2" width="13.54296875"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="2" width="11.0"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="2" width="10.453125"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="2" width="8.54296875"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="2" width="11.81640625"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="2" width="8.26953125"/>
-    <col min="23" max="24" bestFit="true" customWidth="true" style="2" width="22.0"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="2" width="13.1796875"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="2" width="19.453125"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="2" width="23.1796875"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="2" width="19.81640625"/>
-    <col min="29" max="29" customWidth="true" style="2" width="35.26953125"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="2" width="13.1796875"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="2" width="20.453125"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="2" width="15.54296875"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="2" width="24.81640625"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" style="2" width="18.54296875"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" style="2" width="29.453125"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" style="2" width="15.1796875"/>
-    <col min="37" max="39" bestFit="true" customWidth="true" style="2" width="15.54296875"/>
-    <col min="40" max="42" bestFit="true" customWidth="true" style="2" width="10.1796875"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" style="2" width="18.453125"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" style="2" width="18.0"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" style="2" width="13.81640625"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" style="2" width="10.81640625"/>
-    <col min="47" max="47" bestFit="true" customWidth="true" style="2" width="24.54296875"/>
-    <col min="48" max="48" bestFit="true" customWidth="true" style="2" width="10.81640625"/>
-    <col min="49" max="49" bestFit="true" customWidth="true" style="2" width="14.1796875"/>
-    <col min="50" max="50" bestFit="true" customWidth="true" style="2" width="10.81640625"/>
-    <col min="51" max="51" bestFit="true" customWidth="true" style="2" width="12.81640625"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" style="2" width="16.7265625"/>
-    <col min="53" max="16384" style="2" width="8.7265625"/>
+    <col min="1" max="1" width="22.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="22" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="19.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="35.26953125" style="2" customWidth="1"/>
+    <col min="30" max="30" width="13.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="20.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="24.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="18.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="29.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="37" max="39" width="15.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="40" max="42" width="10.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="18.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="18" style="2" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="13.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="10.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="24.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="10.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="14.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="10.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="12.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="16.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="53" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -1676,10 +1666,10 @@
         <v>47</v>
       </c>
       <c r="AR1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AS1" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="AS1" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="AT1" s="2" t="s">
         <v>49</v>
@@ -1706,33 +1696,33 @@
         <v>56</v>
       </c>
       <c r="BB1" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:54" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G2" t="s" s="2">
-        <v>111</v>
+      <c r="G2" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I2" s="2">
         <v>3</v>
@@ -1752,17 +1742,17 @@
       <c r="N2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="O2" t="s" s="2">
-        <v>98</v>
-      </c>
-      <c r="P2" t="s" s="2">
+      <c r="O2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="Q2" t="s" s="2">
-        <v>104</v>
-      </c>
       <c r="R2" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>44</v>
@@ -1774,7 +1764,7 @@
         <v>64</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="W2" s="7">
         <v>10000</v>
@@ -1786,46 +1776,46 @@
         <v>48</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AA2" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="AD2" t="s" s="2">
-        <v>98</v>
+        <v>96</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="AE2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AF2" t="s" s="2">
-        <v>112</v>
+      <c r="AF2" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="AG2" s="2" t="s">
         <v>40</v>
       </c>
       <c r="AH2" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="AI2" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AJ2" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="AL2" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AR2" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AS2" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AT2" s="2" t="s">
         <v>50</v>
@@ -1833,23 +1823,26 @@
       <c r="AU2" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AV2" t="s" s="2">
-        <v>113</v>
+      <c r="AV2" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="AW2" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AX2" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AY2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AZ2" t="s" s="2">
-        <v>114</v>
+      <c r="AZ2" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="BA2" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
+      </c>
+      <c r="BB2" s="2" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1875,61 +1868,61 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="22.26953125"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="20.453125"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" style="2" width="11.1796875"/>
-    <col min="5" max="6" bestFit="true" customWidth="true" style="2" width="13.54296875"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="16.453125"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="6.7265625"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="11.1796875"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="11.81640625"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="9.54296875"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="2" width="7.453125"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="2" width="8.81640625"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="2" width="10.1796875"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="2" width="8.1796875"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="18.453125"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="2" width="13.54296875"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="2" width="11.0"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="2" width="10.453125"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="2" width="8.54296875"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="2" width="11.81640625"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="2" width="10.1796875"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="2" width="22.0"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="2" width="15.7265625"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="2" width="13.1796875"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="2" width="19.453125"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="2" width="23.1796875"/>
-    <col min="28" max="28" customWidth="true" style="2" width="50.54296875"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="2" width="12.1796875"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="2" width="13.1796875"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="2" width="20.453125"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="2" width="15.54296875"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="2" width="24.81640625"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" style="2" width="11.1796875"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" style="2" width="14.54296875"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" style="2" width="11.81640625"/>
-    <col min="37" max="39" bestFit="true" customWidth="true" style="2" width="15.54296875"/>
-    <col min="40" max="42" bestFit="true" customWidth="true" style="2" width="10.1796875"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" style="2" width="18.453125"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" style="2" width="18.0"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" style="2" width="13.81640625"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" style="2" width="10.81640625"/>
-    <col min="47" max="47" bestFit="true" customWidth="true" style="2" width="12.54296875"/>
-    <col min="48" max="48" bestFit="true" customWidth="true" style="2" width="10.81640625"/>
-    <col min="49" max="49" bestFit="true" customWidth="true" style="2" width="14.1796875"/>
-    <col min="50" max="50" bestFit="true" customWidth="true" style="2" width="10.81640625"/>
-    <col min="51" max="51" bestFit="true" customWidth="true" style="2" width="12.81640625"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" style="2" width="16.7265625"/>
-    <col min="53" max="16384" style="2" width="8.7265625"/>
+    <col min="1" max="1" width="22.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="22" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="50.54296875" style="2" customWidth="1"/>
+    <col min="29" max="29" width="12.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="20.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="24.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="11.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="37" max="39" width="15.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="40" max="42" width="10.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="18.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="18" style="2" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="13.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="10.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="12.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="10.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="14.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="10.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="12.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="16.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="53" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:54" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -2055,10 +2048,10 @@
         <v>47</v>
       </c>
       <c r="AR1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AS1" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="AS1" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="AT1" s="2" t="s">
         <v>49</v>
@@ -2085,33 +2078,33 @@
         <v>56</v>
       </c>
       <c r="BB1" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:54" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G2" t="s" s="2">
-        <v>111</v>
+      <c r="G2" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I2" s="2">
         <v>3</v>
@@ -2131,11 +2124,17 @@
       <c r="N2" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="O2" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="P2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>44</v>
@@ -2147,7 +2146,7 @@
         <v>64</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="W2" s="7">
         <v>10000</v>
@@ -2159,43 +2158,46 @@
         <v>48</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AA2" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AC2" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="AE2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AF2" t="s" s="2">
-        <v>112</v>
+      <c r="AF2" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="AG2" s="2" t="s">
         <v>40</v>
       </c>
       <c r="AH2" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="AI2" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AJ2" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="AL2" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AR2" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AS2" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AT2" s="2" t="s">
         <v>50</v>
@@ -2203,23 +2205,26 @@
       <c r="AU2" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AV2" t="s" s="2">
-        <v>113</v>
+      <c r="AV2" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="AW2" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AX2" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AY2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AZ2" t="s" s="2">
-        <v>114</v>
+      <c r="AZ2" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="BA2" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
+      </c>
+      <c r="BB2" s="2" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>